<commit_message>
improved accessibility and ux
</commit_message>
<xml_diff>
--- a/usability_rating.xlsx
+++ b/usability_rating.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertovaldez/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertovaldez/meta-react-capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA3853D-CC94-7A4D-91F3-DEC589F4DD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF55C2DC-1A45-4441-96E3-221633AD84FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{DE46663D-1C1A-484A-8C32-A8A04FF06295}"/>
   </bookViews>
@@ -684,26 +684,26 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
@@ -745,7 +745,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp103.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp104.xml><?xml version="1.0" encoding="utf-8"?>
@@ -813,7 +813,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -825,7 +825,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
@@ -833,7 +833,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,7 +841,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp126.xml><?xml version="1.0" encoding="utf-8"?>
@@ -921,7 +921,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp143.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp144.xml><?xml version="1.0" encoding="utf-8"?>
@@ -937,7 +937,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp147.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp148.xml><?xml version="1.0" encoding="utf-8"?>
@@ -945,7 +945,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp149.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -965,7 +965,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp153.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp154.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1025,7 +1025,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp167.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp168.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1053,7 +1053,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp173.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp174.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1061,7 +1061,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp175.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp176.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1121,7 +1121,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp189.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1133,7 +1133,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp191.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp192.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1141,7 +1141,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp193.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp194.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1277,7 +1277,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp223.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp224.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1285,7 +1285,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp225.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp226.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1293,7 +1293,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp227.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp228.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1301,7 +1301,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp229.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1317,7 +1317,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1329,7 +1329,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1349,7 +1349,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1365,7 +1365,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1409,7 +1409,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1417,7 +1417,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1429,7 +1429,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp51.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp52.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1465,7 +1465,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1473,7 +1473,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp61.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp62.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1509,7 +1509,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1517,7 +1517,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp72.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1525,7 +1525,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp73.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1533,7 +1533,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1541,7 +1541,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp77.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp78.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1553,7 +1553,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1629,7 +1629,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp97.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp98.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1637,7 +1637,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp99.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17287,7 +17287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0060AC88-6094-42D4-81FE-665911260B88}">
   <dimension ref="A2:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -22894,10 +22894,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
@@ -22912,12 +22912,12 @@
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
@@ -22946,10 +22946,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22960,10 +22960,10 @@
       <c r="E13"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
@@ -22976,12 +22976,12 @@
       <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="8" t="s">
         <v>56</v>
       </c>
@@ -22993,16 +22993,16 @@
       <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15"/>
@@ -23020,28 +23020,28 @@
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
       <c r="E23"/>
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23077,16 +23077,16 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
@@ -23121,22 +23121,22 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
     </row>
     <row r="36" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
     </row>
     <row r="37" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
     </row>
     <row r="38" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15"/>
@@ -23165,16 +23165,16 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
     </row>
     <row r="42" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
     </row>
     <row r="43" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15"/>
@@ -23183,10 +23183,10 @@
       <c r="D43" s="15"/>
     </row>
     <row r="44" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
     </row>
     <row r="45" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
@@ -23209,10 +23209,10 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
     </row>
     <row r="48" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="15"/>
@@ -23222,10 +23222,10 @@
       <c r="E48"/>
     </row>
     <row r="49" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
       <c r="E49" s="3"/>
       <c r="K49" s="3"/>
     </row>
@@ -23250,16 +23250,16 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
     </row>
     <row r="53" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
     </row>
     <row r="54" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="15"/>
@@ -23269,13 +23269,13 @@
       <c r="K54" s="3"/>
     </row>
     <row r="55" spans="1:11" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
     </row>
     <row r="56" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
@@ -23289,16 +23289,16 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
     </row>
     <row r="58" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
     </row>
     <row r="59" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15"/>
@@ -23307,13 +23307,51 @@
       <c r="D59" s="15"/>
     </row>
     <row r="60" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="14"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A27:E27"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A10:E10"/>
@@ -23330,59 +23368,12 @@
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:E55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE8B7A03AD6B8242B7625B1FCF791FAE" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c755b74b3a3f26539989579639439fd7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d48761c6-b14a-45e2-9f9a-0b9a919eb093" xmlns:ns3="2341e1b6-22eb-41f1-9523-f4ff41314d71" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b9945f35f5975c6dec86b59cbcceb25" ns2:_="" ns3:_="">
     <xsd:import namespace="d48761c6-b14a-45e2-9f9a-0b9a919eb093"/>
@@ -23619,6 +23610,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -23631,14 +23631,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{797655F4-0189-42F9-8649-1BEB7A5F0460}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F5B9465-ECEA-4836-B0EA-72FD48CA81FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23657,6 +23649,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{797655F4-0189-42F9-8649-1BEB7A5F0460}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{970D41BC-0646-46AA-8E1D-7C1BA02B082F}">
   <ds:schemaRefs>

</xml_diff>